<commit_message>
Text on the excel files of the Tiago folder of the chart.
</commit_message>
<xml_diff>
--- a/Tiago/Exi_Frequency_table_clades.xlsx
+++ b/Tiago/Exi_Frequency_table_clades.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Desktop\VM Shared Folder\Github\DataVis\DataVis2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Desktop\VM Shared Folder\Github\DataVis\DataVis2021\Tiago\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16C123F-9607-4BF4-83E7-B2823E21073C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4337C804-AF02-4E1A-BF2E-BD257A0715AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{24388B20-B62C-40D3-9705-EF5AA6AD371B}"/>
   </bookViews>
@@ -8182,7 +8182,7 @@
               </c:extLst>
               <c:f>'Stacked bar Total Cases'!$F$63:$P$63</c:f>
               <c:numCache>
-                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:formatCode>[$-409]mmm\-\y\y;@</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>43952</c:v>
@@ -8313,7 +8313,7 @@
               </c:extLst>
               <c:f>'Stacked bar Total Cases'!$F$63:$P$63</c:f>
               <c:numCache>
-                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:formatCode>[$-409]mmm\-\y\y;@</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>43952</c:v>
@@ -8441,7 +8441,7 @@
               </c:extLst>
               <c:f>'Stacked bar Total Cases'!$F$63:$P$63</c:f>
               <c:numCache>
-                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:formatCode>[$-409]mmm\-\y\y;@</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>43952</c:v>
@@ -8571,7 +8571,7 @@
               </c:extLst>
               <c:f>'Stacked bar Total Cases'!$F$63:$P$63</c:f>
               <c:numCache>
-                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:formatCode>[$-409]mmm\-\y\y;@</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>43952</c:v>
@@ -8699,7 +8699,7 @@
               </c:extLst>
               <c:f>'Stacked bar Total Cases'!$F$63:$P$63</c:f>
               <c:numCache>
-                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:formatCode>[$-409]mmm\-\y\y;@</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>43952</c:v>
@@ -8827,7 +8827,7 @@
               </c:extLst>
               <c:f>'Stacked bar Total Cases'!$F$63:$P$63</c:f>
               <c:numCache>
-                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:formatCode>[$-409]mmm\-\y\y;@</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>43952</c:v>
@@ -8955,7 +8955,7 @@
               </c:extLst>
               <c:f>'Stacked bar Total Cases'!$F$63:$P$63</c:f>
               <c:numCache>
-                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:formatCode>[$-409]mmm\-\y\y;@</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>43952</c:v>
@@ -9083,7 +9083,7 @@
               </c:extLst>
               <c:f>'Stacked bar Total Cases'!$F$63:$P$63</c:f>
               <c:numCache>
-                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:formatCode>[$-409]mmm\-\y\y;@</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>43952</c:v>
@@ -9211,7 +9211,7 @@
               </c:extLst>
               <c:f>'Stacked bar Total Cases'!$F$63:$P$63</c:f>
               <c:numCache>
-                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:formatCode>[$-409]mmm\-\y\y;@</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>43952</c:v>
@@ -9339,7 +9339,7 @@
               </c:extLst>
               <c:f>'Stacked bar Total Cases'!$F$63:$P$63</c:f>
               <c:numCache>
-                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:formatCode>[$-409]mmm\-\y\y;@</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>43952</c:v>
@@ -9467,7 +9467,7 @@
               </c:extLst>
               <c:f>'Stacked bar Total Cases'!$F$63:$P$63</c:f>
               <c:numCache>
-                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:formatCode>[$-409]mmm\-\y\y;@</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>43952</c:v>
@@ -9595,7 +9595,7 @@
               </c:extLst>
               <c:f>'Stacked bar Total Cases'!$F$63:$P$63</c:f>
               <c:numCache>
-                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:formatCode>[$-409]mmm\-\y\y;@</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>43952</c:v>
@@ -9710,7 +9710,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="[$-409]mmm\-yy;@" sourceLinked="1"/>
+        <c:numFmt formatCode="[$-409]mmm\-\y\y;@" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -10027,7 +10027,7 @@
               </c:extLst>
               <c:f>'Stacked bar Total Cases'!$F$63:$P$63</c:f>
               <c:numCache>
-                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:formatCode>[$-409]mmm\-\y\y;@</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>43952</c:v>
@@ -10158,7 +10158,7 @@
               </c:extLst>
               <c:f>'Stacked bar Total Cases'!$F$63:$P$63</c:f>
               <c:numCache>
-                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:formatCode>[$-409]mmm\-\y\y;@</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>43952</c:v>
@@ -10286,7 +10286,7 @@
               </c:extLst>
               <c:f>'Stacked bar Total Cases'!$F$63:$P$63</c:f>
               <c:numCache>
-                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:formatCode>[$-409]mmm\-\y\y;@</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>43952</c:v>
@@ -10416,7 +10416,7 @@
               </c:extLst>
               <c:f>'Stacked bar Total Cases'!$F$63:$P$63</c:f>
               <c:numCache>
-                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:formatCode>[$-409]mmm\-\y\y;@</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>43952</c:v>
@@ -10544,7 +10544,7 @@
               </c:extLst>
               <c:f>'Stacked bar Total Cases'!$F$63:$P$63</c:f>
               <c:numCache>
-                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:formatCode>[$-409]mmm\-\y\y;@</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>43952</c:v>
@@ -10672,7 +10672,7 @@
               </c:extLst>
               <c:f>'Stacked bar Total Cases'!$F$63:$P$63</c:f>
               <c:numCache>
-                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:formatCode>[$-409]mmm\-\y\y;@</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>43952</c:v>
@@ -10800,7 +10800,7 @@
               </c:extLst>
               <c:f>'Stacked bar Total Cases'!$F$63:$P$63</c:f>
               <c:numCache>
-                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:formatCode>[$-409]mmm\-\y\y;@</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>43952</c:v>
@@ -10928,7 +10928,7 @@
               </c:extLst>
               <c:f>'Stacked bar Total Cases'!$F$63:$P$63</c:f>
               <c:numCache>
-                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:formatCode>[$-409]mmm\-\y\y;@</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>43952</c:v>
@@ -11056,7 +11056,7 @@
               </c:extLst>
               <c:f>'Stacked bar Total Cases'!$F$63:$P$63</c:f>
               <c:numCache>
-                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:formatCode>[$-409]mmm\-\y\y;@</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>43952</c:v>
@@ -11184,7 +11184,7 @@
               </c:extLst>
               <c:f>'Stacked bar Total Cases'!$F$63:$P$63</c:f>
               <c:numCache>
-                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:formatCode>[$-409]mmm\-\y\y;@</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>43952</c:v>
@@ -11312,7 +11312,7 @@
               </c:extLst>
               <c:f>'Stacked bar Total Cases'!$F$63:$P$63</c:f>
               <c:numCache>
-                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:formatCode>[$-409]mmm\-\y\y;@</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>43952</c:v>
@@ -11440,7 +11440,7 @@
               </c:extLst>
               <c:f>'Stacked bar Total Cases'!$F$63:$P$63</c:f>
               <c:numCache>
-                <c:formatCode>[$-409]mmm\-yy;@</c:formatCode>
+                <c:formatCode>[$-409]mmm\-\y\y;@</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>43952</c:v>
@@ -11555,7 +11555,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="[$-409]mmm\-yy;@" sourceLinked="1"/>
+        <c:numFmt formatCode="[$-409]mmm\-yy;@" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -15915,8 +15915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EBEE6B8-6449-4BD3-9780-821FDD19DB72}">
   <dimension ref="A1:S76"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A102" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T111" sqref="T111"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A105" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P126" sqref="P126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>